<commit_message>
Updated data till July 2025
</commit_message>
<xml_diff>
--- a/Spreadsheets/Customer_list.xlsx
+++ b/Spreadsheets/Customer_list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D274"/>
+  <dimension ref="A1:D348"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5917,6 +5917,1486 @@
         </is>
       </c>
     </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>Dollie Desai</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>9825082629</v>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>U2,902 Happy Excellencia, Vesu</t>
+        </is>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>Apr 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>pratik agrwal</t>
+        </is>
+      </c>
+      <c r="B276" t="n">
+        <v>9825291307</v>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>Vesu B201 rajhans cromona</t>
+        </is>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>Apr 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>Leher Thakur</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>9624004792</v>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>C-201, Aakash Evergreen, Vesu</t>
+        </is>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>Apr 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>Aakash Damani</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>7434032409</v>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>Hotel Shreeji Vatika, Piplod, Dumas Road</t>
+        </is>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>Apr 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>Maheshbhai</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>8320999203</v>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>Apr 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>yash</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>8469894517</v>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Apr 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>mamta</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>8000906977</v>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>Vesu JOLLY RECIDANCY</t>
+        </is>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>Apr 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>Suman Kothari</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>9924599987</v>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>Jolly Residency, Vesu</t>
+        </is>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Apr 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>Daljit</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>9898216896</v>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>the grand plaza shop no 16</t>
+        </is>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Apr 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>k.p</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>9012406659</v>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>gourav bagaria</t>
+        </is>
+      </c>
+      <c r="B285" t="n">
+        <v>6291673385</v>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>A/B3 green victory</t>
+        </is>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>yashvi SINGHAN</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>9408120230</v>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>STAR GALAXY G-325</t>
+        </is>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>neha churiwal raj tilak apartment Q206</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>9924624544</v>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>nikita</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>6358107635</v>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>happy glorius G-6-301</t>
+        </is>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>ankita damani</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>8866040899</v>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>Happy Elanza, C1201</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>sapna kothari</t>
+        </is>
+      </c>
+      <c r="B290" t="n">
+        <v>9265764632</v>
+      </c>
+      <c r="C290" t="inlineStr">
+        <is>
+          <t>B401 sapphire court</t>
+        </is>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>kirti gupta</t>
+        </is>
+      </c>
+      <c r="B291" t="n">
+        <v>8347583195</v>
+      </c>
+      <c r="C291" t="inlineStr">
+        <is>
+          <t>vesu someshwar m 80</t>
+        </is>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>diana</t>
+        </is>
+      </c>
+      <c r="B292" t="n">
+        <v>9712902353</v>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>Vesu JOLLY I1203</t>
+        </is>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>kunj bihari</t>
+        </is>
+      </c>
+      <c r="B293" t="n">
+        <v>9651191359</v>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>shiva suwalka</t>
+        </is>
+      </c>
+      <c r="B294" t="n">
+        <v>8875481372</v>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>Vesu aagam hotel nova</t>
+        </is>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>pinki</t>
+        </is>
+      </c>
+      <c r="B295" t="n">
+        <v>8511661008</v>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>shiva suwalka</t>
+        </is>
+      </c>
+      <c r="B296" t="n">
+        <v>7081797878</v>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>Vesu aagam hotel nova 306</t>
+        </is>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>anupama</t>
+        </is>
+      </c>
+      <c r="B297" t="n">
+        <v>9016242079</v>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>jolly H601</t>
+        </is>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>prieet</t>
+        </is>
+      </c>
+      <c r="B298" t="n">
+        <v>9712755116</v>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>rahul baid</t>
+        </is>
+      </c>
+      <c r="B299" t="n">
+        <v>9664951965</v>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>gavtabhai narnave</t>
+        </is>
+      </c>
+      <c r="B300" t="n">
+        <v>7875055627</v>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>hotel sunrise AGAM</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>babita</t>
+        </is>
+      </c>
+      <c r="B301" t="n">
+        <v>8780331212</v>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>rajhans sinfoniya B805</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>chirag shah</t>
+        </is>
+      </c>
+      <c r="B302" t="n">
+        <v>9227907979</v>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>riya</t>
+        </is>
+      </c>
+      <c r="B303" t="n">
+        <v>9460291537</v>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>kassel braun appartment-8C</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>May 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>saloni</t>
+        </is>
+      </c>
+      <c r="B304" t="n">
+        <v>9687422277</v>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>subh anclev A1004</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>mitesh bhai</t>
+        </is>
+      </c>
+      <c r="B305" t="n">
+        <v>9537890657</v>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>dumas</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>janita saluja</t>
+        </is>
+      </c>
+      <c r="B306" t="n">
+        <v>9825107160</v>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>the majestic F 1303</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>zota</t>
+        </is>
+      </c>
+      <c r="B307" t="n">
+        <v>8980878542</v>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>mitushree soni</t>
+        </is>
+      </c>
+      <c r="B308" t="n">
+        <v>9327089115</v>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>althan A1202 marvella residancy</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>renu</t>
+        </is>
+      </c>
+      <c r="B309" t="n">
+        <v>9694966590</v>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>happy glorios G6301</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>sakuntla</t>
+        </is>
+      </c>
+      <c r="B310" t="n">
+        <v>9427344342</v>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>hemtanpark b901</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>sneha juwani</t>
+        </is>
+      </c>
+      <c r="B311" t="n">
+        <v>9638222737</v>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>Fiona A401</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>vandna patel</t>
+        </is>
+      </c>
+      <c r="B312" t="n">
+        <v>9106938198</v>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>dream house102</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>salman salon</t>
+        </is>
+      </c>
+      <c r="B313" t="n">
+        <v>9727182884</v>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>Vesu cannon street 1</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>abhi</t>
+        </is>
+      </c>
+      <c r="B314" t="n">
+        <v>8306540657</v>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>d 301 sangini vedanta</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>jinali</t>
+        </is>
+      </c>
+      <c r="B315" t="n">
+        <v>9555965750</v>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>vesu</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>karishma murarka</t>
+        </is>
+      </c>
+      <c r="B316" t="n">
+        <v>8160833677</v>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>althan D 916 sentosa heights</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>kavita mehta</t>
+        </is>
+      </c>
+      <c r="B317" t="n">
+        <v>9537547555</v>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>The Atmoshphere, Vesu B201</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>Samir Bhai</t>
+        </is>
+      </c>
+      <c r="B318" t="n">
+        <v>9971599922</v>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>Vesu hemton park B301</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>harsh</t>
+        </is>
+      </c>
+      <c r="B319" t="n">
+        <v>7047366468</v>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>vashar preet</t>
+        </is>
+      </c>
+      <c r="B320" t="n">
+        <v>9898169655</v>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>Vesu B2 501 celebrity greens</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>neha shah</t>
+        </is>
+      </c>
+      <c r="B321" t="n">
+        <v>9724198940</v>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>vesu</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>sourav</t>
+        </is>
+      </c>
+      <c r="B322" t="n">
+        <v>9974173433</v>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>jolly A1304</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>shradha jain</t>
+        </is>
+      </c>
+      <c r="B323" t="n">
+        <v>8511031011</v>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>dev raj residancy D801</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>amar singh</t>
+        </is>
+      </c>
+      <c r="B324" t="n">
+        <v>9574802367</v>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>dr abhilasha</t>
+        </is>
+      </c>
+      <c r="B325" t="n">
+        <v>7698173840</v>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>amar singh</t>
+        </is>
+      </c>
+      <c r="B326" t="n">
+        <v>9512504076</v>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>Jun 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>deva park infinity</t>
+        </is>
+      </c>
+      <c r="B327" t="n">
+        <v>7665340302</v>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>ALTHAN</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>mihir</t>
+        </is>
+      </c>
+      <c r="B328" t="n">
+        <v>8108349933</v>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>celebrity greens D2 301</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>himansu</t>
+        </is>
+      </c>
+      <c r="B329" t="n">
+        <v>9818580296</v>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>swapna bhumi D603</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>jayshree vayeda</t>
+        </is>
+      </c>
+      <c r="B330" t="n">
+        <v>8200812058</v>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>Vesu shubhan B1004</t>
+        </is>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>aasha agrwal</t>
+        </is>
+      </c>
+      <c r="B331" t="n">
+        <v>9327922291</v>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>capital green</t>
+        </is>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>ishani</t>
+        </is>
+      </c>
+      <c r="B332" t="n">
+        <v>9723423643</v>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>hampton park B901</t>
+        </is>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>shuruchi</t>
+        </is>
+      </c>
+      <c r="B333" t="n">
+        <v>9687618848</v>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>401 maarquis hitsh</t>
+        </is>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>aagam</t>
+        </is>
+      </c>
+      <c r="B334" t="n">
+        <v>9974842906</v>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>celibrity green B2 501</t>
+        </is>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>foram</t>
+        </is>
+      </c>
+      <c r="B335" t="n">
+        <v>7359724111</v>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>sureshbhai</t>
+        </is>
+      </c>
+      <c r="B336" t="n">
+        <v>7080296220</v>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>falguni</t>
+        </is>
+      </c>
+      <c r="B337" t="n">
+        <v>9586005322</v>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>fiona B1102</t>
+        </is>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>mukesh</t>
+        </is>
+      </c>
+      <c r="B338" t="n">
+        <v>9820019283</v>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>tanish jain</t>
+        </is>
+      </c>
+      <c r="B339" t="n">
+        <v>7984925177</v>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>green vally G415</t>
+        </is>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>Harsha</t>
+        </is>
+      </c>
+      <c r="B340" t="n">
+        <v>9977937276</v>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>priyanshu</t>
+        </is>
+      </c>
+      <c r="B341" t="n">
+        <v>9016717039</v>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>maarqiuis hights 401</t>
+        </is>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>vanita</t>
+        </is>
+      </c>
+      <c r="B342" t="n">
+        <v>9099921981</v>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>poja</t>
+        </is>
+      </c>
+      <c r="B343" t="n">
+        <v>8780113488</v>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>nikunj</t>
+        </is>
+      </c>
+      <c r="B344" t="n">
+        <v>9978062856</v>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>suman</t>
+        </is>
+      </c>
+      <c r="B345" t="n">
+        <v>9327955366</v>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>dream house 203</t>
+        </is>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>rajesh shah</t>
+        </is>
+      </c>
+      <c r="B346" t="n">
+        <v>9825118388</v>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>avi raj</t>
+        </is>
+      </c>
+      <c r="B347" t="n">
+        <v>9664784636</v>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>Vesu</t>
+        </is>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>nirali shah</t>
+        </is>
+      </c>
+      <c r="B348" t="n">
+        <v>9833869913</v>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>piplodd</t>
+        </is>
+      </c>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>Jul 2025</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>